<commit_message>
Correcting an exercise chart on lab 4
</commit_message>
<xml_diff>
--- a/04_pulmonary_shunt/pulmonary_shunt_data.xlsx
+++ b/04_pulmonary_shunt/pulmonary_shunt_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Time</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Art. pO2 (% Norm)</t>
+  </si>
+  <si>
+    <t>***No reset used between the first chart and exercise and heart rate at 0 taken with patient standing. Patient didn’t give up</t>
   </si>
 </sst>
 </file>
@@ -148,12 +151,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -244,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -261,24 +270,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:G32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,7 +605,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
@@ -606,7 +622,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A2" s="7"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -620,7 +636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.75" thickBot="1">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -637,7 +653,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30.75" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -654,7 +670,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30.75" thickBot="1">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -671,7 +687,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30.75" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -688,7 +704,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1">
+    <row r="7" spans="1:5" ht="30.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -705,7 +721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45.75" thickBot="1">
+    <row r="8" spans="1:5" ht="30.75" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -722,7 +738,7 @@
         <v>4618</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30.75" thickBot="1">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -790,7 +806,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45.75" thickBot="1">
+    <row r="13" spans="1:5" ht="30.75" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -807,7 +823,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -841,7 +857,7 @@
         <v>5759</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45.75" thickBot="1">
+    <row r="16" spans="1:5" ht="30.75" thickBot="1">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -858,7 +874,7 @@
         <v>3527</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30.75" thickBot="1">
+    <row r="17" spans="1:12" ht="30.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -875,7 +891,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -892,32 +908,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A20" s="8" t="s">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A21" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3">
@@ -939,178 +955,198 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>0</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>0.02</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>0.04</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>0.06</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>0.08</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="3">
-        <v>99</v>
-      </c>
-      <c r="C23" s="3">
-        <v>144</v>
-      </c>
-      <c r="D23" s="3">
-        <v>161</v>
-      </c>
-      <c r="E23" s="3">
-        <v>196</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="25" spans="1:7" ht="30.75" thickBot="1">
+      <c r="B23" s="5">
+        <v>79</v>
+      </c>
+      <c r="C23" s="5">
+        <v>124</v>
+      </c>
+      <c r="D23" s="5">
+        <v>136</v>
+      </c>
+      <c r="E23" s="5">
+        <v>145</v>
+      </c>
+      <c r="F23" s="5">
+        <v>157</v>
+      </c>
+      <c r="G23" s="5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="25" spans="1:12" ht="30.75" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="11">
-        <v>0.68263888888888891</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30.75" thickBot="1">
+      <c r="B25" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30.75" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="8">
-        <v>8647</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="28" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A28" s="8" t="s">
+      <c r="B26" s="7">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75">
+      <c r="A27" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="30" spans="1:12" ht="30.75" thickBot="1">
+      <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B30" s="8">
         <v>500</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C30" s="8">
         <v>1000</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D30" s="8">
         <v>1500</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E30" s="8">
         <v>2000</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F30" s="8">
         <v>2500</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G30" s="8">
         <v>3000</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A29" s="4" t="s">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B31" s="5">
         <v>100</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C31" s="5">
         <v>100.6</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D31" s="5">
         <v>100.87</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E31" s="5">
         <v>101.2</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F31" s="5">
         <v>103.2</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G31" s="5">
         <v>106.14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A30" s="4" t="s">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B32" s="5">
         <v>0.2</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C32" s="5">
         <v>0.19</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D32" s="5">
         <v>0.18</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E32" s="5">
         <v>0.17</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F32" s="5">
         <v>0.17</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G32" s="5">
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A31" s="4" t="s">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B33" s="5">
         <v>86</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C33" s="5">
         <v>71</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D33" s="5">
         <v>62</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E33" s="5">
         <v>54</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F33" s="5">
         <v>48</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G33" s="5">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A32" s="4" t="s">
+    <row r="34" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B34" s="5">
         <v>94.5</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C34" s="5">
         <v>78</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D34" s="5">
         <v>68.13</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E34" s="5">
         <v>59.3</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F34" s="5">
         <v>52.75</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G34" s="5">
         <v>46.15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing Lab 4 charts
</commit_message>
<xml_diff>
--- a/04_pulmonary_shunt/pulmonary_shunt_data.xlsx
+++ b/04_pulmonary_shunt/pulmonary_shunt_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="42">
   <si>
     <t>Time</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>% Difference</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -270,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -312,11 +315,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -324,16 +327,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -351,63 +358,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -710,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T23" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,19 +729,19 @@
       <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="W2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="19">
         <v>0</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="19">
         <v>10</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="19">
         <v>1</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="19">
         <v>1</v>
       </c>
     </row>
@@ -823,17 +774,17 @@
       <c r="O3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="18"/>
-      <c r="X3" s="3" t="s">
+      <c r="W3" s="21"/>
+      <c r="X3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Z3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AA3" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -866,20 +817,23 @@
         <v>40</v>
       </c>
       <c r="O4" s="5"/>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="X4" s="19">
+      <c r="X4" s="20">
         <f>ABS((B3-L4)/B3)</f>
         <v>2.197802197802198E-2</v>
       </c>
-      <c r="Y4" s="19">
-        <f t="shared" ref="Y4:AA4" si="0">ABS((C3-M4)/C3)</f>
+      <c r="Y4" s="20">
+        <f t="shared" ref="Y4:Z4" si="0">ABS((C3-M4)/C3)</f>
         <v>5.7692307692307696E-2</v>
       </c>
-      <c r="Z4" s="19">
+      <c r="Z4" s="20">
         <f t="shared" si="0"/>
         <v>0.24528301886792453</v>
+      </c>
+      <c r="AA4" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="30.75" thickBot="1">
@@ -911,20 +865,23 @@
         <v>0.183</v>
       </c>
       <c r="O5" s="5"/>
-      <c r="W5" s="15" t="s">
+      <c r="W5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="X5" s="19">
+      <c r="X5" s="20">
         <f t="shared" ref="X5:X19" si="1">ABS((B4-L5)/B4)</f>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="20">
         <f t="shared" ref="Y5:Y19" si="2">ABS((C4-M5)/C4)</f>
         <v>3.3333333333333368E-2</v>
       </c>
-      <c r="Z5" s="19">
+      <c r="Z5" s="20">
         <f t="shared" ref="Z5:Z19" si="3">ABS((D4-N5)/D4)</f>
         <v>1.6666666666666684E-2</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="30.75" thickBot="1">
@@ -956,20 +913,23 @@
         <v>29</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="X6" s="19">
+      <c r="X6" s="20">
         <f t="shared" si="1"/>
         <v>2.4390243902439025E-2</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="20">
         <f t="shared" si="2"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="Z6" s="19">
+      <c r="Z6" s="20">
         <f t="shared" si="3"/>
         <v>0.12121212121212122</v>
+      </c>
+      <c r="AA6" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="30.75" thickBot="1">
@@ -1001,20 +961,23 @@
         <v>0.15</v>
       </c>
       <c r="O7" s="5"/>
-      <c r="W7" s="15" t="s">
+      <c r="W7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="X7" s="19">
+      <c r="X7" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="20">
         <f t="shared" si="2"/>
         <v>1.5384615384615398E-2</v>
       </c>
-      <c r="Z7" s="19">
+      <c r="Z7" s="20">
         <f t="shared" si="3"/>
         <v>7.1428571428571286E-2</v>
+      </c>
+      <c r="AA7" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="45.75" thickBot="1">
@@ -1046,20 +1009,23 @@
         <v>83</v>
       </c>
       <c r="O8" s="5"/>
-      <c r="W8" s="15" t="s">
+      <c r="W8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="19">
+      <c r="X8" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8" s="20">
         <f t="shared" si="2"/>
         <v>4.0404040404040407E-2</v>
       </c>
-      <c r="Z8" s="19">
+      <c r="Z8" s="20">
         <f t="shared" si="3"/>
         <v>0.20192307692307693</v>
+      </c>
+      <c r="AA8" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="45.75" thickBot="1">
@@ -1091,20 +1057,23 @@
         <v>5266</v>
       </c>
       <c r="O9" s="5"/>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X9" s="19">
+      <c r="X9" s="20">
         <f t="shared" si="1"/>
         <v>2.2820800598578377E-2</v>
       </c>
-      <c r="Y9" s="19">
+      <c r="Y9" s="20">
         <f t="shared" si="2"/>
         <v>1.7844396859386152E-3</v>
       </c>
-      <c r="Z9" s="19">
+      <c r="Z9" s="20">
         <f t="shared" si="3"/>
         <v>7.5166842290129959E-2</v>
+      </c>
+      <c r="AA9" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="30.75" thickBot="1">
@@ -1136,20 +1105,23 @@
         <v>72</v>
       </c>
       <c r="O10" s="5"/>
-      <c r="W10" s="15" t="s">
+      <c r="W10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="X10" s="19">
+      <c r="X10" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y10" s="19">
+      <c r="Y10" s="20">
         <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
-      <c r="Z10" s="19">
+      <c r="Z10" s="20">
         <f t="shared" si="3"/>
         <v>8.8607594936708861E-2</v>
+      </c>
+      <c r="AA10" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="30.75" thickBot="1">
@@ -1181,20 +1153,23 @@
         <v>73</v>
       </c>
       <c r="O11" s="5"/>
-      <c r="W11" s="15" t="s">
+      <c r="W11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="X11" s="19">
+      <c r="X11" s="20">
         <f t="shared" si="1"/>
         <v>1.3333333333333334E-2</v>
       </c>
-      <c r="Y11" s="19">
+      <c r="Y11" s="20">
         <f t="shared" si="2"/>
         <v>2.6666666666666668E-2</v>
       </c>
-      <c r="Z11" s="19">
+      <c r="Z11" s="20">
         <f t="shared" si="3"/>
         <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="AA11" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="30.75" thickBot="1">
@@ -1226,20 +1201,23 @@
         <v>1.57</v>
       </c>
       <c r="O12" s="5"/>
-      <c r="W12" s="15" t="s">
+      <c r="W12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="X12" s="19">
+      <c r="X12" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y12" s="19">
+      <c r="Y12" s="20">
         <f t="shared" si="2"/>
         <v>0.10588235294117644</v>
       </c>
-      <c r="Z12" s="19">
+      <c r="Z12" s="20">
         <f t="shared" si="3"/>
         <v>0.12777777777777777</v>
+      </c>
+      <c r="AA12" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="30.75" thickBot="1">
@@ -1271,20 +1249,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="5"/>
-      <c r="W13" s="15" t="s">
+      <c r="W13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="X13" s="19">
+      <c r="X13" s="20">
         <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="Y13" s="19">
+      <c r="Y13" s="20">
         <f t="shared" si="2"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="Z13" s="19">
+      <c r="Z13" s="20">
         <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
+      </c>
+      <c r="AA13" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="45.75" thickBot="1">
@@ -1316,20 +1297,23 @@
         <v>0.97399999999999998</v>
       </c>
       <c r="O14" s="5"/>
-      <c r="W14" s="15" t="s">
+      <c r="W14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X14" s="19">
+      <c r="X14" s="20">
         <f t="shared" si="1"/>
         <v>2.5000000000000022E-2</v>
       </c>
-      <c r="Y14" s="19">
+      <c r="Y14" s="20">
         <f t="shared" si="2"/>
         <v>9.2307692307692382E-2</v>
       </c>
-      <c r="Z14" s="19">
+      <c r="Z14" s="20">
         <f t="shared" si="3"/>
         <v>5.4933333333333332</v>
+      </c>
+      <c r="AA14" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="30.75" thickBot="1">
@@ -1361,20 +1345,23 @@
         <v>493.5</v>
       </c>
       <c r="O15" s="5"/>
-      <c r="W15" s="15" t="s">
+      <c r="W15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="X15" s="19">
+      <c r="X15" s="20">
         <f t="shared" si="1"/>
         <v>0.11428571428571421</v>
       </c>
-      <c r="Y15" s="19">
+      <c r="Y15" s="20">
         <f t="shared" si="2"/>
         <v>3.4117647058823482E-2</v>
       </c>
-      <c r="Z15" s="19">
+      <c r="Z15" s="20">
         <f t="shared" si="3"/>
         <v>0.91972999349381912</v>
+      </c>
+      <c r="AA15" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="30.75" thickBot="1">
@@ -1406,20 +1393,23 @@
         <v>5257</v>
       </c>
       <c r="O16" s="5"/>
-      <c r="W16" s="15" t="s">
+      <c r="W16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="X16" s="19">
+      <c r="X16" s="20">
         <f t="shared" si="1"/>
         <v>1.4779235174579716E-3</v>
       </c>
-      <c r="Y16" s="19">
+      <c r="Y16" s="20">
         <f t="shared" si="2"/>
         <v>2.032144836504711E-3</v>
       </c>
-      <c r="Z16" s="19">
+      <c r="Z16" s="20">
         <f t="shared" si="3"/>
         <v>2.4856241884622519E-2</v>
+      </c>
+      <c r="AA16" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="45.75" thickBot="1">
@@ -1451,20 +1441,23 @@
         <v>2349</v>
       </c>
       <c r="O17" s="5"/>
-      <c r="W17" s="15" t="s">
+      <c r="W17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="X17" s="19">
+      <c r="X17" s="20">
         <f t="shared" si="1"/>
         <v>4.528763769889841E-2</v>
       </c>
-      <c r="Y17" s="19">
+      <c r="Y17" s="20">
         <f t="shared" si="2"/>
         <v>4.528763769889841E-2</v>
       </c>
-      <c r="Z17" s="19">
+      <c r="Z17" s="20">
         <f t="shared" si="3"/>
         <v>4.4733631557543715E-2</v>
+      </c>
+      <c r="AA17" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="30.75" thickBot="1">
@@ -1496,20 +1489,23 @@
         <v>2908</v>
       </c>
       <c r="O18" s="5"/>
-      <c r="W18" s="15" t="s">
+      <c r="W18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X18" s="19">
+      <c r="X18" s="20">
         <f t="shared" si="1"/>
         <v>4.0175557056043212E-2</v>
       </c>
-      <c r="Y18" s="19">
+      <c r="Y18" s="20">
         <f t="shared" si="2"/>
         <v>4.1188386225523295E-2</v>
       </c>
-      <c r="Z18" s="19">
+      <c r="Z18" s="20">
         <f t="shared" si="3"/>
         <v>1.8562267971650354E-2</v>
+      </c>
+      <c r="AA18" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="30.75" thickBot="1">
@@ -1526,20 +1522,23 @@
         <v>45</v>
       </c>
       <c r="O19" s="5"/>
-      <c r="W19" s="15" t="s">
+      <c r="W19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="X19" s="19">
+      <c r="X19" s="20">
         <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="Y19" s="19">
+      <c r="Y19" s="20">
         <f t="shared" si="2"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="Z19" s="19">
+      <c r="Z19" s="20">
         <f t="shared" si="3"/>
         <v>2.1739130434782608E-2</v>
+      </c>
+      <c r="AA19" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="15.75" thickBot="1">
@@ -1626,22 +1625,22 @@
       <c r="W22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="X22" s="8">
+      <c r="X22" s="19">
         <v>500</v>
       </c>
-      <c r="Y22" s="8">
+      <c r="Y22" s="19">
         <v>1000</v>
       </c>
-      <c r="Z22" s="8">
+      <c r="Z22" s="19">
         <v>1500</v>
       </c>
-      <c r="AA22" s="8">
+      <c r="AA22" s="19">
         <v>2000</v>
       </c>
-      <c r="AB22" s="8">
+      <c r="AB22" s="19">
         <v>2500</v>
       </c>
-      <c r="AC22" s="8">
+      <c r="AC22" s="19">
         <v>3000</v>
       </c>
     </row>
@@ -1667,30 +1666,30 @@
       <c r="G23" s="5">
         <v>176</v>
       </c>
-      <c r="W23" s="15" t="s">
+      <c r="W23" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="X23" s="19">
+      <c r="X23" s="20">
         <f>ABS((B31-L32)/B31)</f>
         <v>2.1390374331550728E-2</v>
       </c>
-      <c r="Y23" s="19">
+      <c r="Y23" s="20">
         <f t="shared" ref="Y23:AC23" si="4">ABS((C31-M32)/C31)</f>
         <v>1.8240343347639475E-2</v>
       </c>
-      <c r="Z23" s="19">
+      <c r="Z23" s="20">
         <f t="shared" si="4"/>
         <v>1.3728323699421929E-2</v>
       </c>
-      <c r="AA23" s="19">
+      <c r="AA23" s="20">
         <f t="shared" si="4"/>
         <v>6.4371676462357669E-3</v>
       </c>
-      <c r="AB23" s="19">
+      <c r="AB23" s="20">
         <f t="shared" si="4"/>
         <v>1.8548955153792117E-2</v>
       </c>
-      <c r="AC23" s="19">
+      <c r="AC23" s="20">
         <f t="shared" si="4"/>
         <v>1.4790468364831529E-2</v>
       </c>
@@ -1717,30 +1716,30 @@
       <c r="Q24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="W24" s="15" t="s">
+      <c r="W24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="X24" s="19">
+      <c r="X24" s="20">
         <f t="shared" ref="X24:X26" si="5">ABS((B32-L33)/B32)</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="Y24" s="19">
+      <c r="Y24" s="20">
         <f t="shared" ref="Y24:Y26" si="6">ABS((C32-M33)/C32)</f>
         <v>2.1052631578947385E-2</v>
       </c>
-      <c r="Z24" s="19">
+      <c r="Z24" s="20">
         <f t="shared" ref="Z24:Z26" si="7">ABS((D32-N33)/D32)</f>
         <v>5.2631578947368467E-2</v>
       </c>
-      <c r="AA24" s="19">
+      <c r="AA24" s="20">
         <f t="shared" ref="AA24:AA26" si="8">ABS((E32-O33)/E32)</f>
         <v>3.3333333333333368E-2</v>
       </c>
-      <c r="AB24" s="19">
+      <c r="AB24" s="20">
         <f t="shared" ref="AB24:AB26" si="9">ABS((F32-P33)/F32)</f>
         <v>1.1764705882352951E-2</v>
       </c>
-      <c r="AC24" s="19">
+      <c r="AC24" s="20">
         <f t="shared" ref="AC24:AC26" si="10">ABS((G32-Q33)/G32)</f>
         <v>6.2500000000000056E-3</v>
       </c>
@@ -1773,30 +1772,30 @@
       <c r="Q25" s="3">
         <v>6</v>
       </c>
-      <c r="W25" s="15" t="s">
+      <c r="W25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="X25" s="19">
+      <c r="X25" s="20">
         <f t="shared" si="5"/>
         <v>2.4096385542168676E-2</v>
       </c>
-      <c r="Y25" s="19">
+      <c r="Y25" s="20">
         <f t="shared" si="6"/>
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="Z25" s="19">
+      <c r="Z25" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AA25" s="19">
+      <c r="AA25" s="20">
         <f t="shared" si="8"/>
         <v>5.7692307692307696E-2</v>
       </c>
-      <c r="AB25" s="19">
+      <c r="AB25" s="20">
         <f t="shared" si="9"/>
         <v>0.15217391304347827</v>
       </c>
-      <c r="AC25" s="19">
+      <c r="AC25" s="20">
         <f t="shared" si="10"/>
         <v>0.16666666666666666</v>
       </c>
@@ -1829,30 +1828,30 @@
       <c r="Q26" s="9">
         <v>0.08</v>
       </c>
-      <c r="W26" s="15" t="s">
+      <c r="W26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="X26" s="19">
+      <c r="X26" s="20">
         <f t="shared" si="5"/>
         <v>2.192982456140382E-3</v>
       </c>
-      <c r="Y26" s="19">
+      <c r="Y26" s="20">
         <f t="shared" si="6"/>
         <v>6.2402496099844508E-3</v>
       </c>
-      <c r="Z26" s="19">
+      <c r="Z26" s="20">
         <f t="shared" si="7"/>
         <v>2.1482918096374724E-2</v>
       </c>
-      <c r="AA26" s="19">
+      <c r="AA26" s="20">
         <f t="shared" si="8"/>
         <v>7.7703885194259678E-2</v>
       </c>
-      <c r="AB26" s="19">
+      <c r="AB26" s="20">
         <f t="shared" si="9"/>
         <v>0.1711177052423343</v>
       </c>
-      <c r="AC26" s="19">
+      <c r="AC26" s="20">
         <f t="shared" si="10"/>
         <v>0.18526543878656562</v>
       </c>
@@ -1928,27 +1927,27 @@
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="16">
         <f>0.0935*100</f>
         <v>9.35</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="16">
         <f>100*0.1864</f>
         <v>18.64</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="16">
         <f>100*0.2768</f>
         <v>27.68</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="16">
         <f>100*0.3573</f>
         <v>35.730000000000004</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="16">
         <f>100*0.4259</f>
         <v>42.59</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="16">
         <f>100*0.4868</f>
         <v>48.68</v>
       </c>
@@ -2066,27 +2065,27 @@
       <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="20">
+      <c r="B34" s="16">
         <f>100*0.912</f>
         <v>91.2</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="16">
         <f>100*0.7692</f>
         <v>76.92</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="16">
         <f>100*0.6703</f>
         <v>67.03</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="16">
         <f>100*0.5714</f>
         <v>57.14</v>
       </c>
-      <c r="F34" s="20">
+      <c r="F34" s="16">
         <f>100*0.5055</f>
         <v>50.55</v>
       </c>
-      <c r="G34" s="20">
+      <c r="G34" s="16">
         <f>100*0.4615</f>
         <v>46.150000000000006</v>
       </c>
@@ -2139,7 +2138,7 @@
       <c r="A36" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K36" s="16" t="s">
+      <c r="K36" s="15" t="s">
         <v>39</v>
       </c>
       <c r="L36" s="12"/>
@@ -2157,25 +2156,25 @@
     <mergeCell ref="W2:W3"/>
   </mergeCells>
   <conditionalFormatting sqref="X4:Z19">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23:AC26">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>